<commit_message>
updated fig 3 and table s5
</commit_message>
<xml_diff>
--- a/tables/TableS6_simulated_bloom_design.xlsx
+++ b/tables/TableS6_simulated_bloom_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8E4A4D-5A57-8D42-8DD2-AFE66F9A66F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E884039E-466B-414A-879D-64C404E88976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="560" windowWidth="25600" windowHeight="15540" xr2:uid="{8F65658D-0848-E744-8181-42A1E11BC0FA}"/>
+    <workbookView xWindow="21260" yWindow="6900" windowWidth="25600" windowHeight="15540" xr2:uid="{8F65658D-0848-E744-8181-42A1E11BC0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Formatted" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>Day of peak</t>
   </si>
   <si>
-    <t>Lat of peak</t>
-  </si>
-  <si>
     <t>Peak intensity</t>
   </si>
   <si>
@@ -206,6 +203,9 @@
   </si>
   <si>
     <t>Scenario</t>
+  </si>
+  <si>
+    <t>Lat. of peak</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,13 +614,13 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>29</v>
@@ -647,13 +647,13 @@
         <v>44</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
@@ -673,22 +673,22 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" t="s">
         <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
       </c>
       <c r="I4" t="s">
         <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -705,22 +705,22 @@
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -737,22 +737,22 @@
         <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>